<commit_message>
mnoho změn, předělaný catalogue input + kusovnik, ip moznosti nacitani configu
</commit_message>
<xml_diff>
--- a/TRIMAZKON/TRIMAZKON_address_list.xlsx
+++ b/TRIMAZKON/TRIMAZKON_address_list.xlsx
@@ -451,7 +451,7 @@
         </is>
       </c>
       <c r="E1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2">
@@ -496,7 +496,7 @@
         </is>
       </c>
       <c r="E3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4">
@@ -522,7 +522,7 @@
         </is>
       </c>
       <c r="E4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5">
@@ -542,7 +542,7 @@
         </is>
       </c>
       <c r="E5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6">
@@ -588,7 +588,7 @@
 123TPV456</t>
         </is>
       </c>
-      <c r="E7" t="n">
+      <c r="E7" t="b">
         <v>0</v>
       </c>
     </row>
@@ -608,7 +608,7 @@
           <t>255.255.255.0</t>
         </is>
       </c>
-      <c r="E8" t="n">
+      <c r="E8" t="b">
         <v>0</v>
       </c>
     </row>
@@ -638,7 +638,7 @@
         </is>
       </c>
       <c r="E9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10">
@@ -669,12 +669,12 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>497_Edcha</t>
+          <t>503_Witte</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>172.26.7.240</t>
+          <t>192.168.0.240</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -684,7 +684,18 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>FortiClient Edcha Ex2p78kxp30</t>
+          <t>PC:	10.96.205.175
+NAS:	10.96.205.166
+FH:	10.96.205.154
+	10.96.205.267
+-----------------------------------------
+user:JHV_Vision, omron 
+Pass:*Jhv2708
+---------------------------------------
+FortiClient Austin: 
+Pass:
+1Pm#J@PFIkzM&amp;Q@i 
+UVt1@Ex2p78kxp30atD7we@!qGK</t>
         </is>
       </c>
       <c r="E11" t="n">
@@ -694,20 +705,45 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
+          <t>497_Edcha</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>172.26.7.240</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>FortiClient Edcha Ex2p78kxp30</t>
+        </is>
+      </c>
+      <c r="E12" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
           <t>474 B_Austin</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr">
+      <c r="B13" t="inlineStr">
         <is>
           <t>10.96.205.175</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>255.255.255.0</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
         <is>
           <t>PC:	10.96.205.175
 NAS:	10.96.205.166
@@ -723,27 +759,27 @@
 UVt1@Ex2p78kxp30atD7we@!qGK</t>
         </is>
       </c>
-      <c r="E12" t="n">
+      <c r="E13" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
+    <row r="14">
+      <c r="A14" t="inlineStr">
         <is>
           <t>440_Austin</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr">
+      <c r="B14" t="inlineStr">
         <is>
           <t>10.96.205.240</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>255.255.255.0</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
         <is>
           <t>FortiClient Austin: 
 pass:
@@ -751,42 +787,6 @@
 UVt1@Ex2p78kxp30atD7we@!qGK
 FH-2050-20
 10.96.205.80</t>
-        </is>
-      </c>
-      <c r="E13" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>503_Witte</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>192.168.0.240</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>255.255.255.0</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>PC:	10.96.205.175k
-NAS:	10.96.205.166
-FH:	10.96.205.154
-	10.96.205.267
------------------------------------------
-user:JHV_Vision, omron 
-Pass:*Jhv2708
----------------------------------------
-FortiClient Austin: 
-Pass:
-1Pm#J@PFIkzM&amp;Q@i 
-UVt1@Ex2p78kxp30atD7we@!qGK</t>
         </is>
       </c>
       <c r="E14" t="n">
@@ -804,20 +804,141 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>514_Teleflex</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>192.168.14.240</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>PC:192.168.14.240
+CAM: 192.168.14.??NAS:192.168.14.245
+*******************************
+user: Vision
+pass: *Jhv2708</t>
+        </is>
+      </c>
+      <c r="E1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>518_Valeo II</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>192.168.1.243</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>527_Teijin</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>10.101.28.176</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>XG-X2900:		10.101.28.175
+OP:		10.101.28.117</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>529_Witte</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>192.168.0.240</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Kamera VS-S160MX :192.168.0.18</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Domaci Wifi</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>192.168.1.131</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="E5" t="n">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
@@ -841,11 +962,14 @@
           <t>W</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" t="inlineStr">
         <is>
           <t>\\192.168.0.192\</t>
         </is>
       </c>
+      <c r="D1" t="inlineStr"/>
+      <c r="E1" t="inlineStr"/>
+      <c r="F1" t="inlineStr"/>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -899,57 +1023,117 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>514_Teleflex</t>
+          <t>518_Valeo</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>\\192.168.14.245\Data\Kamery</t>
+          <t>\\192.168.208.200\10_vision</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Vision</t>
+          <t>jhv_vision</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>*Jhv2708</t>
+          <t>Jhv*2708</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>první sít, ixon
+\\192.168.208.200\10_vision</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
+          <t>515_ZF</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Z</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>\\10.9.250.100\08_Project_ZF_515\kamery</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>jhvadmin</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>jhvadm1n</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>514_Teleflex</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>T</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>\\192.168.14.245\Data\Kamery</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Vision</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>*Jhv2708</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
           <t>474_B Austin</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
+      <c r="B7" t="inlineStr">
         <is>
           <t>P</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
+      <c r="C7" t="inlineStr">
         <is>
           <t>\\10.96.205.166\DATA</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
+      <c r="D7" t="inlineStr">
         <is>
           <t>jhv_vision</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr">
+      <c r="E7" t="inlineStr">
         <is>
           <t>*Jhv2708</t>
         </is>
       </c>
-      <c r="F5" t="inlineStr">
+      <c r="F7" t="inlineStr">
         <is>
           <t>10.96.205.166
 VisionNas_474B	
@@ -958,70 +1142,7 @@
         </is>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>515_ZF</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Z</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>\\10.9.250.100\08_Project_ZF_515\kamery</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>jhvadmin</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>jhvadm1n</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>518_Valeo</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>V</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>\\192.168.208.200\10_vision</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>jhv_vision</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>Jhv*2708</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>první sít, ixon
-\\192.168.208.200\10_vision</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C1" r:id="rId1"/>
-  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -1032,14 +1153,87 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>529_Witte</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>192.168.0.240</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Kamera VS-S160MX :192.168.0.18</t>
+        </is>
+      </c>
+      <c r="E1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>515_ZF</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Z</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>\\10.9.250.100\08_Project_ZF_515\kamery</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>jhvadmin</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>jhvadm1n</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Domaci Wifi</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>192.168.1.131</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
prace na ip setting v6, nedodelany manage bin
</commit_message>
<xml_diff>
--- a/TRIMAZKON/TRIMAZKON_address_list.xlsx
+++ b/TRIMAZKON/TRIMAZKON_address_list.xlsx
@@ -416,7 +416,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -427,12 +427,12 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>ddd</t>
+          <t>527_Teijin (1)</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>192.168.000.000</t>
+          <t>10.101.28.176</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
@@ -440,19 +440,27 @@
           <t>255.255.255.0</t>
         </is>
       </c>
-      <c r="E1" t="n">
-        <v>0</v>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>XG-X2900:		10.101.28.17
+OP:		10.101.28.117</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>dddsss</t>
+          <t>474 B_Austin (1)</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>192.168.000.000</t>
+          <t>10.96.205.175</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -460,20 +468,37 @@
           <t>255.255.255.0</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr"/>
-      <c r="E2" t="n">
-        <v>1</v>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>PC:	10.96.205.175
+NAS:	10.96.205.166
+FH:	10.96.205.154
+	10.96.20
+-----------------------------------------
+user:JHV_Vision, omron 
+Pass:*Jhv2708
+---------------------------------------
+FortiClient Austin: 
+Pass:
+1Pm#J@PFIkzM&amp;Q@i 
+UVt1@Ex2p78kxp30atD7we@!qGK</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>xxx</t>
+          <t>527_Teijin (1)</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>192.168.000.000</t>
+          <t>10.101.28.176</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -483,11 +508,203 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>xxxxxxxxxxxxxxxxxxxxxxxx</t>
-        </is>
-      </c>
-      <c r="E3" t="n">
-        <v>0</v>
+          <t>XG-X2900:		10.101.28.17
+OP:		10.101.28.117</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>511_Teleflex</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>192.168.1.242</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Teleflex </t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Domaci Wifi</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>192.168.1.131</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>529_Witte</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>192.168.0.240</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Kamera VS-S160MX :192.168.0.186</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>518_Valeo II</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>192.168.1.243</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>518_Valeo</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>192.168.208.242</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>474 B_Austin</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>10.96.205.175</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>PC:	10.96.
+NAS:	10.96.205.166
+FH:	10.96.205.154
+	10.96.20
+-----------------------------------------
+user:JHV_Vision, omron 
+Pass:*Jhv2708
+---------------------------------------
+FortiClient Austin: 
+Pass:
+1Pm#J@PFIkzM&amp;Q@i 
+UVt1@Ex2p78kxp30atD7we@!qGK</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>527_Teijin</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>10.101.28.176</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>XG-X2900:		10.101.28.17
+OP:		10.101.28.117</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
       </c>
     </row>
   </sheetData>
@@ -501,7 +718,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -512,12 +729,12 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>dddsss</t>
+          <t>515_ZF Stara Boleslav</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>192.168.000.000</t>
+          <t>10.9.250.240</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
@@ -525,7 +742,127 @@
           <t>255.255.255.0</t>
         </is>
       </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>NAS - 10.9.250.100
+User:spravce Pass:Jhv*2708 
+User:jhvadmin Pass:jhvadm1n &gt;&gt;&gt; na portu 8080. 
+123TPV456</t>
+        </is>
+      </c>
       <c r="E1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>527_Teijin</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>10.101.28.176</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>XG-X2900:		10.101.28.175
+OP:		10.101.28.117</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>474 B_Austin</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>10.96.205.175</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>PC:	10.96.205.175
+NAS:	10.96.205.166
+FH:	10.96.205.154
+	10.96.205.245
+-----------------------------------------
+user:JHV_Vision, omron 
+Pass:*Jhv2708
+---------------------------------------
+FortiClient Austin: 
+Pass:
+1Pm#J@PFIkzM&amp;Q@i 
+UVt1@Ex2p78kxp30atD7we@!qGK</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>518_Valeo II</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>192.168.1.243</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>514_Teleflex</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>192.168.14.240</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>PC:192.168.14.240
+CAM: 192.168.14.???
+NAS:192.168.14.245
+*******************************
+user: Vision
+pass: *Jhv2708</t>
+        </is>
+      </c>
+      <c r="E5" t="n">
         <v>1</v>
       </c>
     </row>
@@ -540,14 +877,186 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>514_Teleflex</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>T</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>\\192.168.14.245\Data\Kamery</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Vision</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>*Jhv2708</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Domaci Nas</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>\\192.168.1.20\Data</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>515_ZF</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Z</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>\\10.9.250.100\08_Project_ZF_515\kamery</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>jhvadmin</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>jhvadm1n</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>518_Valeo II</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>\\192.168.1.10\10_vision</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>jhv_vision</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Jhv*2708</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Druha sít, ixon</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>518_Valeo</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>\\192.168.208.200\10_vision</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>jhv_vision</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Jhv*2708</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>první sít, ixon
+\\192.168.208.200\10_vision</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>474_B Austin</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>\\10.96.205.166\DATA</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>jhv_vision</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>*Jhv2708</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>10.96.205.166	
+VisionNas_474B	
+						user:JHV_Vision, omron 
+Pass:*Jhv2708</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -558,7 +1067,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:E2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -566,23 +1075,48 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>dddsss</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>192.168.000.000</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>255.255.255.0</t>
-        </is>
-      </c>
-      <c r="E2" t="b">
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Domaci Wifi</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>192.168.1.131</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="E1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>511_Teleflex</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>192.168.1.242</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Teleflex d</t>
+        </is>
+      </c>
+      <c r="E3" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
dodelany manage bin u ip setting v6
</commit_message>
<xml_diff>
--- a/TRIMAZKON/TRIMAZKON_address_list.xlsx
+++ b/TRIMAZKON/TRIMAZKON_address_list.xlsx
@@ -427,7 +427,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>527_Teijin (1)</t>
+          <t>527_Teijin (2)</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
@@ -442,8 +442,8 @@
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>XG-X2900:		10.101.28.17
-OP:		10.101.28.117</t>
+          <t>XG-X290
+OP:		10.101.28.11</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
@@ -455,20 +455,48 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
+          <t>527_Teijin(1)</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>10.101.28.176</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>XG-X2900:		10.101.28
+OP:		10.101.28.11</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
           <t>474 B_Austin (1)</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="B3" t="inlineStr">
         <is>
           <t>10.96.205.175</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>255.255.255.0</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
         <is>
           <t>PC:	10.96.205.175
 NAS:	10.96.205.166
@@ -484,34 +512,6 @@
 UVt1@Ex2p78kxp30atD7we@!qGK</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>527_Teijin (1)</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>10.101.28.176</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>255.255.255.0</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>XG-X2900:		10.101.28.17
-OP:		10.101.28.117</t>
-        </is>
-      </c>
       <c r="E3" t="inlineStr">
         <is>
           <t>1</t>
@@ -586,7 +586,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Kamera VS-S160MX :192.168.0.186</t>
+          <t>Kamera VS-S160MX :192.168.0.1</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -682,7 +682,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>527_Teijin</t>
+          <t>527_Teijin (1)</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">

</xml_diff>

<commit_message>
práce na ip_v6, spousta oprav
</commit_message>
<xml_diff>
--- a/TRIMAZKON/TRIMAZKON_address_list.xlsx
+++ b/TRIMAZKON/TRIMAZKON_address_list.xlsx
@@ -416,7 +416,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -427,12 +427,12 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>527_Teijin (2)</t>
+          <t>474 B_Austin</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>10.101.28.176</t>
+          <t>10.96.205.175</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
@@ -442,8 +442,7 @@
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>XG-X290
-OP:		10.101.28.11</t>
+          <t>PC:	10.96.aoj</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
@@ -455,12 +454,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>527_Teijin(1)</t>
+          <t>529_Witte55</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>10.101.28.176</t>
+          <t>192.168.0.240</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -470,13 +469,12 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>XG-X2900:		10.101.28
-OP:		10.101.28.11</t>
+          <t>P</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -521,12 +519,12 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>511_Teleflex</t>
+          <t>474 B_Austin (2)</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>192.168.1.242</t>
+          <t>10.96.205.175</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -536,135 +534,12 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t xml:space="preserve">Teleflex </t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Domaci Wifi</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>192.168.1.131</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>255.255.255.0</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr"/>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>529_Witte</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>192.168.0.240</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>255.255.255.0</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>Kamera VS-S160MX :192.168.0.1</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>518_Valeo II</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>192.168.1.243</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>255.255.255.0</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr"/>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>518_Valeo</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>192.168.208.242</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>255.255.255.0</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr"/>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>474 B_Austin</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>10.96.205.175</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>255.255.255.0</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>PC:	10.96.
+          <t>10.96.205.1
 NAS:	10.96.205.166
 FH:	10.96.205.154
 	10.96.20
 -----------------------------------------
-user:JHV_Vision, omron 
+user:JHV_Vision, omron llllllllllllll
 Pass:*Jhv2708
 ---------------------------------------
 FortiClient Austin: 
@@ -673,16 +548,157 @@
 UVt1@Ex2p78kxp30atD7we@!qGK</t>
         </is>
       </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>474 B_Austin (2) (1)</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>10.96.205.175</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>10.96.205.1
+NAS:	10.96.205.166
+FH:	10.96.205.154
+	10.96.20
+-----------------------------------------
+user:JHV_Vision, omron llllllllllllll
+Pass:*Jhv2708
+---------------------------------------
+FortiClient Austin: 
+Pass:
+1Pm#J@PFIkzM&amp;Q@i 
+UVt1@Ex2p78kxp30atD7we@!qGK</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>529_Witte</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>192.168.0.240</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>47</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>10.96.205.175</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>PC:	10.96.205.</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>518_Val</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>192.168.208.242</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>518_Valeo II</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>192.168.1.243</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>ssssssss</t>
+        </is>
+      </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>527_Teijin (1)</t>
+          <t>527_</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -697,13 +713,86 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>XG-X2900:		10.101.28.17
-OP:		10.101.28.117</t>
+          <t>PC:	10.96.20</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Dom</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>192.168.1.131</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
           <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>474 B_A</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>10.96.205.175</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>dfddddddddddddddddd
+adf
+afd
+afsdfaadfs</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Domac</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>192.168.1.13</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
moznost manualniho nastavovani ip pres tray, zmeny u disků z ip, možnost pridavat dalsi projekty
</commit_message>
<xml_diff>
--- a/TRIMAZKON/TRIMAZKON_address_list.xlsx
+++ b/TRIMAZKON/TRIMAZKON_address_list.xlsx
@@ -416,7 +416,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -427,22 +427,17 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>474 B_Austin</t>
+          <t>xz</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>10.96.205.175</t>
+          <t>192.168.000.000</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
           <t>255.255.255.0</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>PC:	10.96.aoj</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
@@ -454,12 +449,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>529_Witte55</t>
+          <t>474 B_Austin</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>192.168.0.240</t>
+          <t>10.96.205.175</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -469,32 +464,59 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>P</t>
+          <t>PC:	10.96.aoj</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
+          <t>529_Witte55</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>192.168.0.240</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
           <t>474 B_Austin (1)</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="B4" t="inlineStr">
         <is>
           <t>10.96.205.175</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>255.255.255.0</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
         <is>
           <t>PC:	10.96.205.175
 NAS:	10.96.205.166
@@ -507,32 +529,33 @@
 FortiClient Austin: 
 Pass:
 1Pm#J@PFIkzM&amp;Q@i 
-UVt1@Ex2p78kxp30atD7we@!qGK</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
+UVt1@Ex2p78kxp30atD7we@!qGK
+dfa</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
+    <row r="5">
+      <c r="A5" t="inlineStr">
         <is>
           <t>474 B_Austin (2)</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="B5" t="inlineStr">
         <is>
           <t>10.96.205.175</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>255.255.255.0</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
         <is>
           <t>10.96.205.1
 NAS:	10.96.205.166
@@ -548,29 +571,29 @@
 UVt1@Ex2p78kxp30atD7we@!qGK</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
         <is>
           <t>474 B_Austin (2) (1)</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
+      <c r="B6" t="inlineStr">
         <is>
           <t>10.96.205.175</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>255.255.255.0</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
         <is>
           <t>10.96.205.1
 NAS:	10.96.205.166
@@ -583,34 +606,8 @@
 FortiClient Austin: 
 Pass:
 1Pm#J@PFIkzM&amp;Q@i 
-UVt1@Ex2p78kxp30atD7we@!qGK</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>529_Witte</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>192.168.0.240</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>255.255.255.0</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>PC</t>
+UVt1@Ex2p78kxp30atD7we@!qGK
+af</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -622,12 +619,12 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>47</t>
+          <t>529_Witte</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>10.96.205.175</t>
+          <t>192.168.0.240</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -637,24 +634,24 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>PC:	10.96.205.</t>
+          <t>PC</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>518_Val</t>
+          <t>Domac</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>192.168.208.242</t>
+          <t>192.168.1.13</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -671,12 +668,12 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>518_Valeo II</t>
+          <t>47</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>192.168.1.243</t>
+          <t>10.96.205.175</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -686,34 +683,30 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>ssssssss</t>
+          <t>PC:	10.96.205.
+asdf</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>527_</t>
+          <t>518_Val</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>10.101.28.176</t>
+          <t>192.168.208.242</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
           <t>255.255.255.0</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>PC:	10.96.20</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -725,12 +718,12 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Dom</t>
+          <t>518_Valeo II</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>192.168.1.131</t>
+          <t>192.168.1.243</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -738,29 +731,83 @@
           <t>255.255.255.0</t>
         </is>
       </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>ssssssss</t>
+        </is>
+      </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
+          <t>527_</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>10.101.28.176</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>PC:	10.96.20</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Dom</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>192.168.1.131</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
           <t>474 B_A</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr">
+      <c r="B14" t="inlineStr">
         <is>
           <t>10.96.205.175</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>255.255.255.0</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
         <is>
           <t>dfddddddddddddddddd
 adf
@@ -768,29 +815,7 @@
 afsdfaadfs</t>
         </is>
       </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>Domac</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>192.168.1.13</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>255.255.255.0</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
+      <c r="E14" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1021,34 +1046,39 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>515_ZF</t>
+          <t>518_Valeo II</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Z</t>
+          <t>V</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>\\10.9.250.100\08_Project_ZF_515\kamery</t>
+          <t>\\192.168.1.10\10_vision</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>jhvadmin</t>
+          <t>jhv_vision</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>jhvadm1n</t>
+          <t>Jhv*2708</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Druha sít, ixon</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>518_Valeo II</t>
+          <t>518_Valeo</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -1058,7 +1088,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>\\192.168.1.10\10_vision</t>
+          <t>\\192.168.208.200\10_vision</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -1073,24 +1103,26 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Druha sít, ixon</t>
+          <t>první sít, ixon
+\\192.168.208.200\10_vision
+sadf</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>518_Valeo</t>
+          <t>474_B Austin</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>P</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>\\192.168.208.200\10_vision</t>
+          <t>\\10.96.205.166\DATA</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -1100,48 +1132,43 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Jhv*2708</t>
+          <t>*Jhv2708</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
-        <is>
-          <t>první sít, ixon
-\\192.168.208.200\10_vision</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>474_B Austin</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>P</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>\\10.96.205.166\DATA</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>jhv_vision</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>*Jhv2708</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
         <is>
           <t>10.96.205.166	
 VisionNas_474B	
 						user:JHV_Vision, omron 
-Pass:*Jhv2708</t>
+Pass:*Jhv2708
+adf</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>515_ZF</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Z</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>\\10.9.250.100\08_Project_ZF_515\kamery</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>jhvadmin</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>jhvadm1n</t>
         </is>
       </c>
     </row>
@@ -1156,7 +1183,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1184,28 +1211,28 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
+    <row r="2">
+      <c r="A2" t="inlineStr">
         <is>
           <t>511_Teleflex</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="B2" t="inlineStr">
         <is>
           <t>192.168.1.242</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>255.255.255.0</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
         <is>
           <t>Teleflex d</t>
         </is>
       </c>
-      <c r="E3" t="b">
+      <c r="E2" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
testovani tooltipu, par oprav, predelani disku na objekt logiku
</commit_message>
<xml_diff>
--- a/TRIMAZKON/TRIMAZKON_address_list.xlsx
+++ b/TRIMAZKON/TRIMAZKON_address_list.xlsx
@@ -416,7 +416,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -427,12 +427,12 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>xz</t>
+          <t>533valeo</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>192.168.000.000</t>
+          <t>192.168.227.27</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
@@ -442,19 +442,19 @@
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>474 B_Austin</t>
+          <t>529_Witte</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>10.96.205.175</t>
+          <t>192.168.0.240</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -464,7 +464,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>PC:	10.96.aoj</t>
+          <t>Kamera VS-S160MX :192.168.0.18</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -476,12 +476,12 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>529_Witte55</t>
+          <t>527_Teijin</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>192.168.0.240</t>
+          <t>10.101.28.176</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -491,7 +491,8 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>P</t>
+          <t>XG-X2900:		10.101.28.175
+OP:		10.101.28.117</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -503,12 +504,12 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>474 B_Austin (1)</t>
+          <t>518_Valeo II</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>10.96.205.175</t>
+          <t>192.168.1.243</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -516,12 +517,112 @@
           <t>255.255.255.0</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>518_Valeo</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>192.168.208.242</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>515_ZF Stara kkkBoleslav</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>10.9.250.240</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>NAS - 10.9.250.100Uer:spravce Pass:Jhv*2708 
+User:jhvadmin Pass
+123TPV456</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>511_Teleflex</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>192.168.1.242</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Teleflex d</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>503_Witte</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>192.168.0.240</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
         <is>
           <t>PC:	10.96.205.175
 NAS:	10.96.205.166
 FH:	10.96.205.154
-	10.96.20
+	10.96.205.267
 -----------------------------------------
 user:JHV_Vision, omron 
 Pass:*Jhv2708
@@ -529,40 +630,97 @@
 FortiClient Austin: 
 Pass:
 1Pm#J@PFIkzM&amp;Q@i 
-UVt1@Ex2p78kxp30atD7we@!qGK
-dfa</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
+UVt1@Ex2p78kxp30atD7we@!qGK</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>514_Teleflex</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>192.168.14.240</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>PC:192.168.14.240
+CAM: 192.168.14.??NAS:192.168.14.245
+*******************************
+user: Vision
+pass: *Jhv2708</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>474 B_Austin (2)</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>497_Edcha</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>172.26.7.240</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>FortiClient Edcha Ex2p78kxp30</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>474 B_Austin</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
         <is>
           <t>10.96.205.175</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>255.255.255.0</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>10.96.205.1
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>PC:	10.96.205.175
 NAS:	10.96.205.166
 FH:	10.96.205.154
-	10.96.20
+	10.96.205.245
 -----------------------------------------
-user:JHV_Vision, omron llllllllllllll
+user:JHV_Vision, omron 
 Pass:*Jhv2708
 ---------------------------------------
 FortiClient Austin: 
@@ -571,251 +729,39 @@
 UVt1@Ex2p78kxp30atD7we@!qGK</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr">
+      <c r="E11" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>474 B_Austin (2) (1)</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>10.96.205.175</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>255.255.255.0</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>10.96.205.1
-NAS:	10.96.205.166
-FH:	10.96.205.154
-	10.96.20
------------------------------------------
-user:JHV_Vision, omron llllllllllllll
-Pass:*Jhv2708
----------------------------------------
-FortiClient Austin: 
-Pass:
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>440_Austin</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>10.96.205.240</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>FortiClient Austin: 
+pass:
 1Pm#J@PFIkzM&amp;Q@i 
 UVt1@Ex2p78kxp30atD7we@!qGK
-af</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>529_Witte</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>192.168.0.240</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>255.255.255.0</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>PC</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Domac</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>192.168.1.13</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>255.255.255.0</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>47</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>10.96.205.175</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>255.255.255.0</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>PC:	10.96.205.
-asdf</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>518_Val</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>192.168.208.242</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>255.255.255.0</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>518_Valeo II</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>192.168.1.243</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>255.255.255.0</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>ssssssss</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>527_</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>10.101.28.176</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>255.255.255.0</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>PC:	10.96.20</t>
+FH-2050-20
+10.96.205.80</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>Dom</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>192.168.1.131</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>255.255.255.0</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>474 B_A</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>10.96.205.175</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>255.255.255.0</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>dfddddddddddddddddd
-adf
-afd
-afsdfaadfs</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -991,7 +937,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1002,27 +948,17 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>514_Teleflex</t>
+          <t>witte</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>\\192.168.14.245\Data\Kamery</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>Vision</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>*Jhv2708</t>
+          <t>\\192.168.0.192\</t>
         </is>
       </c>
     </row>
@@ -1104,71 +1040,96 @@
       <c r="F4" t="inlineStr">
         <is>
           <t>první sít, ixon
-\\192.168.208.200\10_vision
-sadf</t>
+\\192.168.208.200\10_vision</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
+          <t>515_ZF</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Z</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>\\10.9.250.100\08_Project_ZF_515\kamery</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>jhvadmin</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>jhvadm1n</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>514_Teleflex</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>T</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>\\192.168.14.245\Data\Kamery</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Vision</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>*Jhv2708</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
           <t>474_B Austin</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
+      <c r="B7" t="inlineStr">
         <is>
           <t>P</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
+      <c r="C7" t="inlineStr">
         <is>
           <t>\\10.96.205.166\DATA</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
+      <c r="D7" t="inlineStr">
         <is>
           <t>jhv_vision</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr">
+      <c r="E7" t="inlineStr">
         <is>
           <t>*Jhv2708</t>
         </is>
       </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>10.96.205.166	
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>10.96.205.166
 VisionNas_474B	
 						user:JHV_Vision, omron 
-Pass:*Jhv2708
-adf</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>515_ZF</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Z</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>\\10.9.250.100\08_Project_ZF_515\kamery</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>jhvadmin</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>jhvadm1n</t>
+Pass:*Jhv2708</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
práce na nove vizualizaci, tooltip, catalogue
</commit_message>
<xml_diff>
--- a/TRIMAZKON/TRIMAZKON_address_list.xlsx
+++ b/TRIMAZKON/TRIMAZKON_address_list.xlsx
@@ -427,12 +427,12 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>533valeo</t>
+          <t>529_Witte</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>192.168.227.27</t>
+          <t>192.168.0.240</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
@@ -440,21 +440,26 @@
           <t>255.255.255.0</t>
         </is>
       </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Kamera VS-S160MX :192.168.0.18</t>
+        </is>
+      </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>529_Witte</t>
+          <t>440_Austin</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>192.168.0.240</t>
+          <t>10.96.205.240</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -464,24 +469,29 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Kamera VS-S160MX :192.168.0.18</t>
+          <t>FortiClient Austin: 
+pass:
+1Pm#J@PFIkzM&amp;Q@i 
+UVt1@Ex2p78kxp30atD7we@!qGK
+FH-2050-20
+10.96.205.80</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>527_Teijin</t>
+          <t>474 B_Austin</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>10.101.28.176</t>
+          <t>10.96.205.175</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -491,8 +501,18 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>XG-X2900:		10.101.28.175
-OP:		10.101.28.117</t>
+          <t>PC:	10.96.205.175
+NAS:	10.96.205.166
+FH:	10.96.205.154
+	10.96.205.245
+-----------------------------------------
+user:JHV_Vision, omron 
+Pass:*Jhv2708
+---------------------------------------
+FortiClient Austin: 
+Pass:
+1Pm#J@PFIkzM&amp;Q@i 
+UVt1@Ex2p78kxp30atD7we@!qGK</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -504,12 +524,12 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>518_Valeo II</t>
+          <t>497_Edcha</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>192.168.1.243</t>
+          <t>172.26.7.240</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -517,21 +537,26 @@
           <t>255.255.255.0</t>
         </is>
       </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>FortiClient Edcha Ex2p78kxp30</t>
+        </is>
+      </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>518_Valeo</t>
+          <t>503_Witte</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>192.168.208.242</t>
+          <t>192.168.0.240</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -539,85 +564,7 @@
           <t>255.255.255.0</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>515_ZF Stara kkkBoleslav</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>10.9.250.240</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>255.255.255.0</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>NAS - 10.9.250.100Uer:spravce Pass:Jhv*2708 
-User:jhvadmin Pass
-123TPV456</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>511_Teleflex</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>192.168.1.242</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>255.255.255.0</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>Teleflex d</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>503_Witte</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>192.168.0.240</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>255.255.255.0</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
+      <c r="D5" t="inlineStr">
         <is>
           <t>PC:	10.96.205.175
 NAS:	10.96.205.166
@@ -633,29 +580,56 @@
 UVt1@Ex2p78kxp30atD7we@!qGK</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr">
+      <c r="E5" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>511_Teleflex</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>192.168.1.242</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Teleflex d</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
         <is>
           <t>514_Teleflex</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
+      <c r="B7" t="inlineStr">
         <is>
           <t>192.168.14.240</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>255.255.255.0</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
         <is>
           <t>PC:192.168.14.240
 CAM: 192.168.14.??NAS:192.168.14.245
@@ -664,21 +638,73 @@
 pass: *Jhv2708</t>
         </is>
       </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>515_ZF Stara kkkBoleslav</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>10.9.250.240</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>NAS - 10.9.250.100Uer:spravce Pass:Jhv*2708 
+User:jhvadmin Pass
+123TPV456</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>518_Valeo</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>192.168.208.242</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr"/>
       <c r="E9" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>497_Edcha</t>
+          <t>518_Valeo II</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>172.26.7.240</t>
+          <t>192.168.1.243</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -686,26 +712,22 @@
           <t>255.255.255.0</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>FortiClient Edcha Ex2p78kxp30</t>
-        </is>
-      </c>
+      <c r="D10" t="inlineStr"/>
       <c r="E10" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>474 B_Austin</t>
+          <t>527_Teijin</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>10.96.205.175</t>
+          <t>10.101.28.176</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -715,18 +737,8 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>PC:	10.96.205.175
-NAS:	10.96.205.166
-FH:	10.96.205.154
-	10.96.205.245
------------------------------------------
-user:JHV_Vision, omron 
-Pass:*Jhv2708
----------------------------------------
-FortiClient Austin: 
-Pass:
-1Pm#J@PFIkzM&amp;Q@i 
-UVt1@Ex2p78kxp30atD7we@!qGK</t>
+          <t>XG-X2900:		10.101.28.175
+OP:		10.101.28.117</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -738,12 +750,12 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>440_Austin</t>
+          <t>533valeo</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>10.96.205.240</t>
+          <t>192.168.227.27</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -751,16 +763,7 @@
           <t>255.255.255.0</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>FortiClient Austin: 
-pass:
-1Pm#J@PFIkzM&amp;Q@i 
-UVt1@Ex2p78kxp30atD7we@!qGK
-FH-2050-20
-10.96.205.80</t>
-        </is>
-      </c>
+      <c r="D12" t="inlineStr"/>
       <c r="E12" t="inlineStr">
         <is>
           <t>0</t>
@@ -948,153 +951,153 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>witte</t>
+          <t>514_Teleflex</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>\\192.168.0.192\</t>
+          <t>\\192.168.14.245\Data\Kamery</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Vision</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>*Jhv2708</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Domaci Nas</t>
+          <t>witte</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>S</t>
+          <t>W</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>\\192.168.1.20\Data</t>
+          <t>\\192.168.0.192\</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>518_Valeo II</t>
+          <t>Domaci Nas</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>S</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>\\192.168.1.10\10_vision</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>jhv_vision</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>Jhv*2708</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>Druha sít, ixon</t>
+          <t>\\192.168.1.20\Data</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
+          <t>518_Valeo II</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>\\192.168.1.10\10_vision</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>jhv_vision</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Jhv*2708</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Druha sít, ixon</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
           <t>518_Valeo</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="B5" t="inlineStr">
         <is>
           <t>V</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
+      <c r="C5" t="inlineStr">
         <is>
           <t>\\192.168.208.200\10_vision</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
+      <c r="D5" t="inlineStr">
         <is>
           <t>jhv_vision</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
+      <c r="E5" t="inlineStr">
         <is>
           <t>Jhv*2708</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr">
+      <c r="F5" t="inlineStr">
         <is>
           <t>první sít, ixon
 \\192.168.208.200\10_vision</t>
         </is>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>515_ZF</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Z</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>\\10.9.250.100\08_Project_ZF_515\kamery</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>jhvadmin</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>jhvadm1n</t>
-        </is>
-      </c>
-    </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>514_Teleflex</t>
+          <t>515_ZF</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>Z</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>\\192.168.14.245\Data\Kamery</t>
+          <t>\\10.9.250.100\08_Project_ZF_515\kamery</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Vision</t>
+          <t>jhvadmin</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>*Jhv2708</t>
+          <t>jhvadm1n</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
opravy a loading animace
</commit_message>
<xml_diff>
--- a/TRIMAZKON/TRIMAZKON_address_list.xlsx
+++ b/TRIMAZKON/TRIMAZKON_address_list.xlsx
@@ -427,12 +427,12 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>529_Witte</t>
+          <t>533valeo</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>192.168.0.240</t>
+          <t>192.168.227.27</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
@@ -440,34 +440,58 @@
           <t>255.255.255.0</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>Kamera VS-S160MX :192.168.0.18</t>
-        </is>
-      </c>
+      <c r="D1" t="inlineStr"/>
       <c r="E1" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
+          <t>527_Teijin</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>10.101.28.176</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>XG-X2900:		10.101.28.175
+OP:		10.101.28.117</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
           <t>440_Austin</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="B3" t="inlineStr">
         <is>
           <t>10.96.205.240</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>255.255.255.0</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
         <is>
           <t>FortiClient Austin: 
 pass:
@@ -477,29 +501,29 @@
 10.96.205.80</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="E3" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
+    <row r="4">
+      <c r="A4" t="inlineStr">
         <is>
           <t>474 B_Austin</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="B4" t="inlineStr">
         <is>
           <t>10.96.205.175</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>255.255.255.0</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
         <is>
           <t>PC:	10.96.205.175
 NAS:	10.96.205.166
@@ -515,33 +539,6 @@
 UVt1@Ex2p78kxp30atD7we@!qGK</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>497_Edcha</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>172.26.7.240</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>255.255.255.0</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>FortiClient Edcha Ex2p78kxp30</t>
-        </is>
-      </c>
       <c r="E4" t="inlineStr">
         <is>
           <t>0</t>
@@ -551,20 +548,47 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
+          <t>497_Edcha</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>172.26.7.240</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>FortiClient Edcha Ex2p78kxp30</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
           <t>503_Witte</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
+      <c r="B6" t="inlineStr">
         <is>
           <t>192.168.0.240</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>255.255.255.0</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
         <is>
           <t>PC:	10.96.205.175
 NAS:	10.96.205.166
@@ -580,33 +604,6 @@
 UVt1@Ex2p78kxp30atD7we@!qGK</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>511_Teleflex</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>192.168.1.242</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>255.255.255.0</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>Teleflex d</t>
-        </is>
-      </c>
       <c r="E6" t="inlineStr">
         <is>
           <t>0</t>
@@ -616,20 +613,47 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
+          <t>511_Teleflex</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>192.168.1.242</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Teleflex d</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
           <t>514_Teleflex</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
+      <c r="B8" t="inlineStr">
         <is>
           <t>192.168.14.240</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>255.255.255.0</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
         <is>
           <t>PC:192.168.14.240
 CAM: 192.168.14.??NAS:192.168.14.245
@@ -638,57 +662,35 @@
 pass: *Jhv2708</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr">
+      <c r="E8" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
+    <row r="9">
+      <c r="A9" t="inlineStr">
         <is>
           <t>515_ZF Stara kkkBoleslav</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr">
+      <c r="B9" t="inlineStr">
         <is>
           <t>10.9.250.240</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>255.255.255.0</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
         <is>
           <t>NAS - 10.9.250.100Uer:spravce Pass:Jhv*2708 
 User:jhvadmin Pass
 123TPV456</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>518_Valeo</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>192.168.208.242</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>255.255.255.0</t>
-        </is>
-      </c>
       <c r="E9" t="inlineStr">
         <is>
           <t>0</t>
@@ -698,12 +700,12 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>518_Valeo II</t>
+          <t>518_Valeo</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>192.168.1.243</t>
+          <t>192.168.208.242</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -711,21 +713,22 @@
           <t>255.255.255.0</t>
         </is>
       </c>
+      <c r="D10" t="inlineStr"/>
       <c r="E10" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>527_Teijin</t>
+          <t>518_Valeo II</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>10.101.28.176</t>
+          <t>192.168.1.243</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -733,27 +736,22 @@
           <t>255.255.255.0</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>XG-X2900:		10.101.28.175
-OP:		10.101.28.117</t>
-        </is>
-      </c>
+      <c r="D11" t="inlineStr"/>
       <c r="E11" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>533valeo</t>
+          <t>529_Witte</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>192.168.227.27</t>
+          <t>192.168.0.240</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -761,9 +759,14 @@
           <t>255.255.255.0</t>
         </is>
       </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Kamera VS-S160MX :192.168.0.18</t>
+        </is>
+      </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -937,7 +940,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -948,183 +951,222 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>514_Teleflex</t>
+          <t>Info JHV</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>I</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>\\192.168.14.245\Data\Kamery</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>Vision</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>*Jhv2708</t>
+          <t>\\FS-1\Infojhv</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>witte</t>
+          <t>solution</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>L</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>\\192.168.0.192\</t>
+          <t>\\FS-1\Solutions-Aktivni\</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>jakub.hlavacek@jhv.cz</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Domaci Nas</t>
+          <t>514_Teleflex</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>S</t>
+          <t>T</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>\\192.168.1.20\Data</t>
+          <t>\\192.168.14.245\Data\Kamery</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Vision</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>*Jhv2708</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>518_Valeo II</t>
+          <t>witte</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>\\192.168.1.10\10_vision</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>jhv_vision</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>Jhv*2708</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>Druha sít, ixon</t>
+          <t>\\192.168.0.192\</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
+          <t>Domaci Nas</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>\\192.168.1.20\Data</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>518_Valeo II</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>\\192.168.1.10\10_vision</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>jhv_vision</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Jhv*2708</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Druha sít, ixon</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
           <t>518_Valeo</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
+      <c r="B7" t="inlineStr">
         <is>
           <t>V</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
+      <c r="C7" t="inlineStr">
         <is>
           <t>\\192.168.208.200\10_vision</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
+      <c r="D7" t="inlineStr">
         <is>
           <t>jhv_vision</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr">
+      <c r="E7" t="inlineStr">
         <is>
           <t>Jhv*2708</t>
         </is>
       </c>
-      <c r="F5" t="inlineStr">
+      <c r="F7" t="inlineStr">
         <is>
           <t>první sít, ixon
 \\192.168.208.200\10_vision</t>
         </is>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
+    <row r="8">
+      <c r="A8" t="inlineStr">
         <is>
           <t>515_ZF</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
+      <c r="B8" t="inlineStr">
         <is>
           <t>Z</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
+      <c r="C8" t="inlineStr">
         <is>
           <t>\\10.9.250.100\08_Project_ZF_515\kamery</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
+      <c r="D8" t="inlineStr">
         <is>
           <t>jhvadmin</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr">
+      <c r="E8" t="inlineStr">
         <is>
           <t>jhvadm1n</t>
         </is>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
+    <row r="9">
+      <c r="A9" t="inlineStr">
         <is>
           <t>474_B Austin</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
+      <c r="B9" t="inlineStr">
         <is>
           <t>P</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
+      <c r="C9" t="inlineStr">
         <is>
           <t>\\10.96.205.166\DATA</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
+      <c r="D9" t="inlineStr">
         <is>
           <t>jhv_vision</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr">
+      <c r="E9" t="inlineStr">
         <is>
           <t>*Jhv2708</t>
         </is>
       </c>
-      <c r="F7" t="inlineStr">
+      <c r="F9" t="inlineStr">
         <is>
           <t>10.96.205.166
 VisionNas_474B	

</xml_diff>